<commit_message>
Location based recommendation with the euclidean distance
</commit_message>
<xml_diff>
--- a/Data/Cleaned data.xlsx
+++ b/Data/Cleaned data.xlsx
@@ -586,7 +586,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Mental Health Services, General and Preventive Care</t>
+          <t>General and Preventive Care, Mental Health Services</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Diagnostic and Imaging Services, Treatment and Procedures, Pediatric Care, Rehabilitation and Therapy</t>
+          <t>Diagnostic and Imaging Services, Rehabilitation and Therapy, Treatment and Procedures, Pediatric Care</t>
         </is>
       </c>
     </row>
@@ -736,7 +736,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Emergency and Critical Care, Treatment and Procedures, Rehabilitation and Therapy</t>
+          <t>Rehabilitation and Therapy, Emergency and Critical Care, Treatment and Procedures</t>
         </is>
       </c>
     </row>
@@ -811,7 +811,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Emergency and Critical Care, Neonatal Care, Oncology, Women's Health, Diagnostic and Imaging Services, Treatment and Procedures</t>
+          <t>Women's Health, Treatment and Procedures, Neonatal Care, Diagnostic and Imaging Services, Emergency and Critical Care, Oncology</t>
         </is>
       </c>
     </row>
@@ -886,7 +886,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Palliative and Supportive Care, Oncology</t>
+          <t>Oncology, Palliative and Supportive Care</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Emergency and Critical Care, Orthopedics, General and Preventive Care, Women's Health, Diagnostic and Imaging Services, Treatment and Procedures, Pediatric Care</t>
+          <t>Women's Health, Orthopedics, Treatment and Procedures, Pediatric Care, Diagnostic and Imaging Services, Emergency and Critical Care, General and Preventive Care</t>
         </is>
       </c>
     </row>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>Ophthalmology, Mental Health Services, Dermatology, Emergency and Critical Care, Orthopedics, General and Preventive Care, ENT (Ear, Nose, Throat), Infectious Diseases, Patient Care, Rehabilitation and Therapy, Diagnostic and Imaging Services, Treatment and Procedures</t>
+          <t>Ophthalmology, Orthopedics, Rehabilitation and Therapy, Treatment and Procedures, Mental Health Services, Dermatology, ENT (Ear, Nose, Throat), Diagnostic and Imaging Services, Emergency and Critical Care, Infectious Diseases, General and Preventive Care, Patient Care</t>
         </is>
       </c>
     </row>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>Mental Health Services, Patient Care, Emergency and Critical Care</t>
+          <t>Emergency and Critical Care, Mental Health Services, Patient Care</t>
         </is>
       </c>
     </row>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>Ophthalmology, Emergency and Critical Care, Neonatal Care, Orthopedics, Infectious Diseases, Women's Health, Patient Care, Rehabilitation and Therapy</t>
+          <t>Ophthalmology, Women's Health, Orthopedics, Rehabilitation and Therapy, Neonatal Care, Emergency and Critical Care, Infectious Diseases, Patient Care</t>
         </is>
       </c>
     </row>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>General and Preventive Care, Infectious Diseases, Women's Health, Patient Care, Treatment and Procedures</t>
+          <t>Women's Health, Treatment and Procedures, Infectious Diseases, General and Preventive Care, Patient Care</t>
         </is>
       </c>
     </row>
@@ -3244,7 +3244,7 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>Treatment and Procedures, General and Preventive Care, Emergency and Critical Care</t>
+          <t>Treatment and Procedures, Emergency and Critical Care, General and Preventive Care</t>
         </is>
       </c>
     </row>
@@ -3311,7 +3311,7 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>Women's Health, Treatment and Procedures, Patient Care, Infectious Diseases</t>
+          <t>Infectious Diseases, Treatment and Procedures, Patient Care, Women's Health</t>
         </is>
       </c>
     </row>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>Women's Health, General and Preventive Care</t>
+          <t>General and Preventive Care, Women's Health</t>
         </is>
       </c>
     </row>
@@ -3449,7 +3449,7 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>General and Preventive Care, Emergency and Critical Care</t>
+          <t>Emergency and Critical Care, General and Preventive Care</t>
         </is>
       </c>
     </row>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>Ophthalmology, Orthopedics, Infectious Diseases, Patient Care, Diagnostic and Imaging Services</t>
+          <t>Ophthalmology, Orthopedics, Diagnostic and Imaging Services, Infectious Diseases, Patient Care</t>
         </is>
       </c>
     </row>
@@ -3794,7 +3794,7 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>Women's Health, Treatment and Procedures, Patient Care, Rehabilitation and Therapy</t>
+          <t>Rehabilitation and Therapy, Patient Care, Treatment and Procedures, Women's Health</t>
         </is>
       </c>
     </row>

</xml_diff>